<commit_message>
Falta acabar uns textos nos resultados. Falta esquema com a BPB/BTB
</commit_message>
<xml_diff>
--- a/L2_Latex/AAC_Lab2.xlsx
+++ b/L2_Latex/AAC_Lab2.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>CPI</t>
   </si>
@@ -53,6 +53,16 @@
   <si>
     <t>Delay Slot 
 Usage (%)</t>
+  </si>
+  <si>
+    <t>Speed Up</t>
+  </si>
+  <si>
+    <t>Jump 
+Miss Rate  (%)</t>
+  </si>
+  <si>
+    <t># Jumps</t>
   </si>
 </sst>
 </file>
@@ -86,7 +96,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -114,6 +124,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -148,19 +164,6 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -178,32 +181,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -212,15 +216,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -235,15 +230,6 @@
     <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -253,10 +239,79 @@
     <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -462,7 +517,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Folha1!$H$4:$H$10</c:f>
+              <c:f>Folha1!$J$4:$J$10</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
@@ -599,7 +654,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Folha1!$H$11:$H$21</c:f>
+              <c:f>Folha1!$J$11:$J$21</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="11"/>
@@ -607,31 +662,31 @@
                   <c:v>1.2437046521553563</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.2210840802390097</c:v>
+                  <c:v>1.1826717883055911</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.1984635083226634</c:v>
+                  <c:v>1.1600512163892445</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.1754161331626121</c:v>
+                  <c:v>1.1370038412291934</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.1527955612462655</c:v>
+                  <c:v>1.1143832693128468</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.1297481860862142</c:v>
+                  <c:v>1.0913358941527955</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.1071276141698676</c:v>
+                  <c:v>1.0687153222364489</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.0840802390098165</c:v>
+                  <c:v>1.0456679470763979</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.0614596670934699</c:v>
+                  <c:v>1.0230473751600513</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.0384122919334187</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>1.3619866284622733</c:v>
@@ -739,7 +794,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Folha1!$H$21:$H$27</c:f>
+              <c:f>Folha1!$J$21:$J$27</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
@@ -747,22 +802,168 @@
                   <c:v>1.3619866284622733</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.3132760267430754</c:v>
+                  <c:v>1.2483285577841452</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.2636103151862463</c:v>
+                  <c:v>1.1986628462273161</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.2139446036294175</c:v>
+                  <c:v>1.148997134670487</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.1642788920725884</c:v>
+                  <c:v>1.0993314231136582</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.1146131805157593</c:v>
+                  <c:v>1.0496657115568291</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.0649474689589302</c:v>
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Teste 4</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent4">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent4">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent4">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Folha1!$C$28:$C$37</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0" formatCode="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.111111111111111</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22.222222222222221</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>33.333333333333336</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44.444444444444443</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>55.555555555555557</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>66.666666666666671</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>77.777777777777771</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>88.888888888888886</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="0">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Folha1!$J$28:$J$37</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1.6472828401836266</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5419299718283197</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.4741886630781609</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.4064473543280021</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.3387062946643187</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.2709649859141599</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.203223677164001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.1354826175003176</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.0677413087501588</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -777,11 +978,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="313022552"/>
-        <c:axId val="313023336"/>
+        <c:axId val="243796064"/>
+        <c:axId val="243791360"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="313022552"/>
+        <c:axId val="243796064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -900,13 +1101,13 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="313023336"/>
+        <c:crossAx val="243791360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="10"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="313023336"/>
+        <c:axId val="243791360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.8"/>
@@ -1014,7 +1215,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="313022552"/>
+        <c:crossAx val="243796064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1273,7 +1474,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Folha1!$I$4:$I$10</c:f>
+              <c:f>Folha1!$K$4:$K$10</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="7"/>
@@ -1311,11 +1512,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="354218256"/>
-        <c:axId val="354218648"/>
+        <c:axId val="243791752"/>
+        <c:axId val="243794888"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="354218256"/>
+        <c:axId val="243791752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -1429,12 +1630,12 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="354218648"/>
+        <c:crossAx val="243794888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="354218648"/>
+        <c:axId val="243794888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1541,7 +1742,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="354218256"/>
+        <c:crossAx val="243791752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="3.0000000000000009E-3"/>
@@ -1680,7 +1881,7 @@
           <c:spPr>
             <a:ln w="9525" cap="rnd">
               <a:solidFill>
-                <a:srgbClr val="FFC000"/>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -1697,17 +1898,11 @@
             <c:size val="6"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="40000"/>
-                  <a:lumOff val="60000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:ln w="9525" cap="rnd">
                 <a:solidFill>
-                  <a:schemeClr val="accent2">
-                    <a:lumMod val="40000"/>
-                    <a:lumOff val="60000"/>
-                  </a:schemeClr>
+                  <a:srgbClr val="FF0000"/>
                 </a:solidFill>
                 <a:round/>
               </a:ln>
@@ -1761,7 +1956,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Folha1!$I$11:$I$20</c:f>
+              <c:f>Folha1!$K$11:$K$20</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1769,31 +1964,31 @@
                   <c:v>11.477411477411477</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11.26865965575643</c:v>
+                  <c:v>10.914175430304462</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11.059907834101383</c:v>
+                  <c:v>10.705423608649415</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10.847217298830202</c:v>
+                  <c:v>10.492733073378234</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10.638465477175155</c:v>
+                  <c:v>10.283981251723187</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10.425774941903974</c:v>
+                  <c:v>10.071290716452006</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10.217023120248927</c:v>
+                  <c:v>9.8625388947969608</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10.004332584977746</c:v>
+                  <c:v>9.6498483595257802</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.7955807633226986</c:v>
+                  <c:v>9.441096537870731</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9.582890228051518</c:v>
+                  <c:v>9.2284060025995505</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1808,11 +2003,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="354221000"/>
-        <c:axId val="354215120"/>
+        <c:axId val="243795280"/>
+        <c:axId val="243796456"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="354221000"/>
+        <c:axId val="243795280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -1926,15 +2121,16 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="354215120"/>
+        <c:crossAx val="243796456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="10"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="354215120"/>
+        <c:axId val="243796456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="9"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2039,7 +2235,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="354221000"/>
+        <c:crossAx val="243795280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2170,8 +2366,8 @@
           <c:spPr>
             <a:ln w="9525" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent6">
-                  <a:lumMod val="75000"/>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="50000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -2189,14 +2385,14 @@
             <c:size val="6"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent6">
-                  <a:lumMod val="75000"/>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="50000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:ln w="9525" cap="rnd">
                 <a:solidFill>
-                  <a:schemeClr val="accent6">
-                    <a:lumMod val="75000"/>
+                  <a:schemeClr val="bg1">
+                    <a:lumMod val="50000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:round/>
@@ -2242,7 +2438,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Folha1!$I$21:$I$27</c:f>
+              <c:f>Folha1!$K$21:$K$27</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="7"/>
@@ -2250,22 +2446,22 @@
                   <c:v>5.6166056166056171</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.4157312221828349</c:v>
+                  <c:v>5.1478986962857931</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.2109181141439205</c:v>
+                  <c:v>4.9430855882468787</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.0061050061050061</c:v>
+                  <c:v>4.7382724802079643</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.8012918980660917</c:v>
+                  <c:v>4.533459372169049</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.5964787900271773</c:v>
+                  <c:v>4.3286462641301346</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.3916656819882629</c:v>
+                  <c:v>4.1238331560912211</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2280,11 +2476,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="354215904"/>
-        <c:axId val="354219040"/>
+        <c:axId val="419515640"/>
+        <c:axId val="419517208"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="354215904"/>
+        <c:axId val="419515640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="100"/>
@@ -2398,12 +2594,12 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="354219040"/>
+        <c:crossAx val="419517208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="354219040"/>
+        <c:axId val="419517208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="4"/>
@@ -2511,9 +2707,496 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="354215904"/>
+        <c:crossAx val="419515640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-PT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-PT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="pt-PT"/>
+              <a:t>Execution Time vs Delay Slot Usage - Teste 4</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-PT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+              <a:ln w="9525" cap="rnd">
+                <a:solidFill>
+                  <a:srgbClr val="FFC000"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Folha1!$C$28:$C$37</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0" formatCode="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.111111111111111</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22.222222222222221</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>33.333333333333336</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>44.444444444444443</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>55.555555555555557</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>66.666666666666671</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>77.777777777777771</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>88.888888888888886</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="0">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Folha1!$K$28:$K$37</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>26047.88294143133</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24381.976446492576</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>23310.80783016267</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22239.639213832761</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>21168.474536216472</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20097.305919886563</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>19026.137303556658</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>17954.972625940365</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16883.80400961046</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>15812.635393280556</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="419516032"/>
+        <c:axId val="419516424"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="419516032"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="100"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-PT"/>
+                  <a:t>Delay Slot Usage (%)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-PT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="419516424"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="419516424"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="15000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="pt-PT"/>
+                  <a:t>Execution Time (µs)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="pt-PT"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="419516032"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:dispUnits>
+          <c:builtInUnit val="thousands"/>
+        </c:dispUnits>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -2720,6 +3403,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="343">
   <cs:axisTitle>
@@ -4728,20 +5451,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="343">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>877047</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>168338</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>114246</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>188348</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>541405</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>54038</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>660666</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>74048</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4763,15 +5988,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1901</xdr:colOff>
-      <xdr:row>49</xdr:row>
-      <xdr:rowOff>178828</xdr:rowOff>
+      <xdr:colOff>452537</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>86780</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>824843</xdr:colOff>
-      <xdr:row>64</xdr:row>
-      <xdr:rowOff>64528</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>394608</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>162980</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4792,13 +6017,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>140590</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>53406</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
+      <xdr:col>27</xdr:col>
       <xdr:colOff>303737</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>129606</xdr:rowOff>
@@ -4822,13 +6047,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>154466</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>122576</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
+      <xdr:col>27</xdr:col>
       <xdr:colOff>296488</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>8276</xdr:rowOff>
@@ -4845,6 +6070,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>190499</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>166686</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Gráfico 8"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -5116,9 +6371,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:AJ27"/>
+  <dimension ref="B3:AN74"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="E12" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M45" sqref="M45"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5126,849 +6383,1345 @@
     <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.42578125" customWidth="1"/>
     <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" customWidth="1"/>
+    <col min="10" max="10" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13" customWidth="1"/>
+    <col min="13" max="14" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:36" ht="30" x14ac:dyDescent="0.25">
-      <c r="B3" s="5" t="s">
+    <row r="3" spans="2:40" ht="45" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="I3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="K3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="L3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="M3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B4" s="7">
+    <row r="4" spans="2:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="21">
         <v>1</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="4">
         <v>0</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="4">
         <v>59</v>
       </c>
-      <c r="E4" s="8">
-        <f t="shared" ref="E4:E27" si="0">D4+F4+G4</f>
+      <c r="E4" s="4">
+        <f t="shared" ref="E4:E27" si="0">D4+F4+H4</f>
         <v>65</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="4">
         <v>6</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="21">
+        <v>7</v>
+      </c>
+      <c r="H4" s="30">
         <v>0</v>
       </c>
-      <c r="H4" s="9">
-        <f t="shared" ref="H4:H10" si="1">E4/D4</f>
+      <c r="I4" s="26">
+        <f>(H4/G4)*100</f>
+        <v>0</v>
+      </c>
+      <c r="J4" s="5">
+        <f t="shared" ref="J4:J10" si="1">E4/D4</f>
         <v>1.1016949152542372</v>
       </c>
-      <c r="I4" s="10">
-        <f t="shared" ref="I4:I27" si="2">(E4/(253.89*10^9))*10^9</f>
+      <c r="K4" s="6">
+        <f t="shared" ref="K4:K37" si="2">(E4/(253.89*10^9))*10^9</f>
         <v>0.2560163850486431</v>
       </c>
-      <c r="J4" s="2">
+      <c r="L4" s="6">
+        <f>$K$4/K4</f>
+        <v>1</v>
+      </c>
+      <c r="M4" s="25">
         <v>253.89</v>
       </c>
-      <c r="AH4" s="1">
+      <c r="AL4" s="1">
         <f>0*10</f>
         <v>0</v>
       </c>
-      <c r="AJ4">
-        <f xml:space="preserve"> F11 - F11*0.01*C12</f>
+      <c r="AN4">
+        <f t="shared" ref="AN4:AN15" si="3" xml:space="preserve"> F11 - F11*0.01*C12</f>
         <v>427.55555555555554</v>
       </c>
     </row>
-    <row r="5" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B5" s="11"/>
-      <c r="C5" s="8">
+    <row r="5" spans="2:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="21"/>
+      <c r="C5" s="4">
         <v>16.670000000000002</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="4">
         <v>59</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="4">
         <f t="shared" si="0"/>
         <v>64</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F5" s="4">
         <v>5</v>
       </c>
-      <c r="G5" s="8">
-        <v>0</v>
-      </c>
-      <c r="H5" s="9">
+      <c r="G5" s="21"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="5">
         <f t="shared" si="1"/>
         <v>1.0847457627118644</v>
       </c>
-      <c r="I5" s="10">
+      <c r="K5" s="6">
         <f t="shared" si="2"/>
         <v>0.25207767143251014</v>
       </c>
-      <c r="J5" s="3"/>
-      <c r="AH5">
+      <c r="L5" s="6">
+        <f t="shared" ref="L5:L10" si="4">$K$4/K5</f>
+        <v>1.015625</v>
+      </c>
+      <c r="M5" s="25"/>
+      <c r="AL5">
         <f>100</f>
         <v>100</v>
       </c>
-      <c r="AJ5">
-        <f xml:space="preserve"> F12 - F12*0.01*C13</f>
+      <c r="AN5">
+        <f t="shared" si="3"/>
         <v>332.88888888888891</v>
       </c>
     </row>
-    <row r="6" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B6" s="11"/>
-      <c r="C6" s="8">
+    <row r="6" spans="2:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="21"/>
+      <c r="C6" s="4">
         <v>33.299999999999997</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="4">
         <v>59</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="4">
         <f t="shared" si="0"/>
         <v>63</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="4">
         <v>4</v>
       </c>
-      <c r="G6" s="8">
-        <v>0</v>
-      </c>
-      <c r="H6" s="9">
+      <c r="G6" s="21"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="26"/>
+      <c r="J6" s="5">
         <f t="shared" si="1"/>
         <v>1.0677966101694916</v>
       </c>
-      <c r="I6" s="10">
+      <c r="K6" s="6">
         <f t="shared" si="2"/>
         <v>0.24813895781637718</v>
       </c>
-      <c r="J6" s="3"/>
-      <c r="AH6">
+      <c r="L6" s="6">
+        <f t="shared" si="4"/>
+        <v>1.0317460317460316</v>
+      </c>
+      <c r="M6" s="25"/>
+      <c r="AL6">
         <v>200</v>
       </c>
-      <c r="AJ6">
-        <f xml:space="preserve"> F13 - F13*0.01*C14</f>
+      <c r="AN6">
+        <f t="shared" si="3"/>
         <v>250</v>
       </c>
     </row>
-    <row r="7" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B7" s="11"/>
-      <c r="C7" s="8">
+    <row r="7" spans="2:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="21"/>
+      <c r="C7" s="4">
         <v>50</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="4">
         <v>59</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="4">
         <f t="shared" si="0"/>
         <v>62</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F7" s="4">
         <v>3</v>
       </c>
-      <c r="G7" s="8">
-        <v>0</v>
-      </c>
-      <c r="H7" s="9">
+      <c r="G7" s="21"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="26"/>
+      <c r="J7" s="5">
         <f t="shared" si="1"/>
         <v>1.0508474576271187</v>
       </c>
-      <c r="I7" s="10">
+      <c r="K7" s="6">
         <f t="shared" si="2"/>
         <v>0.24420024420024419</v>
       </c>
-      <c r="J7" s="3"/>
-      <c r="AH7">
+      <c r="L7" s="6">
+        <f t="shared" si="4"/>
+        <v>1.0483870967741935</v>
+      </c>
+      <c r="M7" s="25"/>
+      <c r="AL7">
         <v>300</v>
       </c>
-      <c r="AJ7">
-        <f xml:space="preserve"> F14 - F14*0.01*C15</f>
+      <c r="AN7">
+        <f t="shared" si="3"/>
         <v>178.33333333333334</v>
       </c>
     </row>
-    <row r="8" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B8" s="11"/>
-      <c r="C8" s="8">
+    <row r="8" spans="2:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="21"/>
+      <c r="C8" s="4">
         <v>66.599999999999994</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="4">
         <v>59</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="4">
         <f t="shared" si="0"/>
         <v>61</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8" s="4">
         <v>2</v>
       </c>
-      <c r="G8" s="8">
-        <v>0</v>
-      </c>
-      <c r="H8" s="9">
+      <c r="G8" s="21"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="5">
         <f t="shared" si="1"/>
         <v>1.0338983050847457</v>
       </c>
-      <c r="I8" s="10">
+      <c r="K8" s="6">
         <f t="shared" si="2"/>
         <v>0.2402615305841112</v>
       </c>
-      <c r="J8" s="3"/>
-      <c r="AH8">
+      <c r="L8" s="6">
+        <f t="shared" si="4"/>
+        <v>1.0655737704918034</v>
+      </c>
+      <c r="M8" s="25"/>
+      <c r="AL8">
         <v>400</v>
       </c>
-      <c r="AJ8">
-        <f xml:space="preserve"> F15 - F15*0.01*C16</f>
+      <c r="AN8">
+        <f t="shared" si="3"/>
         <v>119.11111111111109</v>
       </c>
     </row>
-    <row r="9" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B9" s="11"/>
-      <c r="C9" s="8">
+    <row r="9" spans="2:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="21"/>
+      <c r="C9" s="4">
         <v>83.3</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D9" s="4">
         <v>59</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9" s="4">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F9" s="4">
         <v>1</v>
       </c>
-      <c r="G9" s="8">
-        <v>0</v>
-      </c>
-      <c r="H9" s="9">
+      <c r="G9" s="21"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="5">
         <f t="shared" si="1"/>
         <v>1.0169491525423728</v>
       </c>
-      <c r="I9" s="10">
+      <c r="K9" s="6">
         <f t="shared" si="2"/>
         <v>0.23632281696797827</v>
       </c>
-      <c r="J9" s="3"/>
-      <c r="AH9">
-        <f>AH8+100</f>
+      <c r="L9" s="6">
+        <f t="shared" si="4"/>
+        <v>1.0833333333333333</v>
+      </c>
+      <c r="M9" s="25"/>
+      <c r="AL9">
+        <f>AL8+100</f>
         <v>500</v>
       </c>
-      <c r="AJ9">
-        <f xml:space="preserve"> F16 - F16*0.01*C17</f>
+      <c r="AN9">
+        <f t="shared" si="3"/>
         <v>71.333333333333314</v>
       </c>
     </row>
-    <row r="10" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B10" s="12"/>
-      <c r="C10" s="8">
+    <row r="10" spans="2:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="21"/>
+      <c r="C10" s="4">
         <v>100</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D10" s="4">
         <v>59</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10" s="4">
         <f t="shared" si="0"/>
         <v>59</v>
       </c>
-      <c r="F10" s="8">
+      <c r="F10" s="4">
         <v>0</v>
       </c>
-      <c r="G10" s="8">
-        <v>0</v>
-      </c>
-      <c r="H10" s="8">
+      <c r="G10" s="21"/>
+      <c r="H10" s="32"/>
+      <c r="I10" s="26"/>
+      <c r="J10" s="4">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="I10" s="10">
+      <c r="K10" s="6">
         <f t="shared" si="2"/>
         <v>0.23238410335184528</v>
       </c>
-      <c r="J10" s="3"/>
-      <c r="AH10">
-        <f t="shared" ref="AH10:AH15" si="3">AH9+100</f>
+      <c r="L10" s="6">
+        <f t="shared" si="4"/>
+        <v>1.1016949152542372</v>
+      </c>
+      <c r="M10" s="25"/>
+      <c r="AL10">
+        <f t="shared" ref="AL10:AL15" si="5">AL9+100</f>
         <v>600</v>
       </c>
-      <c r="AJ10">
-        <f xml:space="preserve"> F17 - F17*0.01*C18</f>
+      <c r="AN10">
+        <f t="shared" si="3"/>
         <v>35.777777777777786</v>
       </c>
     </row>
-    <row r="11" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B11" s="13">
+    <row r="11" spans="2:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="23">
         <v>2</v>
       </c>
-      <c r="C11" s="14">
-        <f>AH4/9</f>
+      <c r="C11" s="7">
+        <f t="shared" ref="C11:C19" si="6">AL4/9</f>
         <v>0</v>
       </c>
-      <c r="D11" s="15">
+      <c r="D11" s="8">
         <v>2343</v>
       </c>
-      <c r="E11" s="15">
+      <c r="E11" s="8">
         <f t="shared" si="0"/>
         <v>2914</v>
       </c>
-      <c r="F11" s="15">
+      <c r="F11" s="8">
         <v>481</v>
       </c>
-      <c r="G11" s="15">
+      <c r="G11" s="23">
+        <v>523</v>
+      </c>
+      <c r="H11" s="33">
         <v>90</v>
       </c>
-      <c r="H11" s="16">
-        <f t="shared" ref="H11:H27" si="4" xml:space="preserve"> E11/D11</f>
+      <c r="I11" s="27">
+        <f>(H11/G11)*100</f>
+        <v>17.208413001912046</v>
+      </c>
+      <c r="J11" s="9">
+        <f t="shared" ref="J11:J27" si="7" xml:space="preserve"> E11/D11</f>
         <v>1.2437046521553563</v>
       </c>
-      <c r="I11" s="17">
+      <c r="K11" s="10">
         <f t="shared" si="2"/>
         <v>11.477411477411477</v>
       </c>
-      <c r="J11" s="3"/>
-      <c r="AH11">
+      <c r="L11" s="10">
+        <f>$K$11/K11</f>
+        <v>1</v>
+      </c>
+      <c r="M11" s="25"/>
+      <c r="AL11">
+        <f t="shared" si="5"/>
+        <v>700</v>
+      </c>
+      <c r="AN11">
         <f t="shared" si="3"/>
-        <v>700</v>
-      </c>
-      <c r="AJ11">
-        <f xml:space="preserve"> F18 - F18*0.01*C19</f>
         <v>11.888888888888886</v>
       </c>
     </row>
-    <row r="12" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B12" s="18"/>
-      <c r="C12" s="16">
-        <f>AH5/9</f>
+    <row r="12" spans="2:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="23"/>
+      <c r="C12" s="9">
+        <f t="shared" si="6"/>
         <v>11.111111111111111</v>
       </c>
-      <c r="D12" s="15">
+      <c r="D12" s="8">
         <v>2343</v>
       </c>
-      <c r="E12" s="15">
+      <c r="E12" s="8">
         <f t="shared" si="0"/>
-        <v>2861</v>
-      </c>
-      <c r="F12" s="15">
-        <f t="shared" ref="F12:F19" si="5">ROUNDUP($F$11 -$F$11*0.01*C12,0)</f>
+        <v>2771</v>
+      </c>
+      <c r="F12" s="8">
+        <f t="shared" ref="F12:F19" si="8">ROUNDUP($F$11 -$F$11*0.01*C12,0)</f>
         <v>428</v>
       </c>
-      <c r="G12" s="15">
-        <v>90</v>
-      </c>
-      <c r="H12" s="16">
-        <f t="shared" si="4"/>
-        <v>1.2210840802390097</v>
-      </c>
-      <c r="I12" s="17">
+      <c r="G12" s="23"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="9">
+        <f t="shared" si="7"/>
+        <v>1.1826717883055911</v>
+      </c>
+      <c r="K12" s="10">
         <f t="shared" si="2"/>
-        <v>11.26865965575643</v>
-      </c>
-      <c r="J12" s="3"/>
-      <c r="AH12">
+        <v>10.914175430304462</v>
+      </c>
+      <c r="L12" s="10">
+        <f t="shared" ref="L12:L20" si="9">$K$11/K12</f>
+        <v>1.051605918440996</v>
+      </c>
+      <c r="M12" s="25"/>
+      <c r="AL12">
+        <f t="shared" si="5"/>
+        <v>800</v>
+      </c>
+      <c r="AN12">
         <f t="shared" si="3"/>
-        <v>800</v>
-      </c>
-      <c r="AJ12">
-        <f xml:space="preserve"> F19 - F19*0.01*C20</f>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B13" s="18"/>
-      <c r="C13" s="16">
-        <f>AH6/9</f>
+    <row r="13" spans="2:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="23"/>
+      <c r="C13" s="9">
+        <f t="shared" si="6"/>
         <v>22.222222222222221</v>
       </c>
-      <c r="D13" s="15">
+      <c r="D13" s="8">
         <v>2343</v>
       </c>
-      <c r="E13" s="15">
+      <c r="E13" s="8">
         <f t="shared" si="0"/>
-        <v>2808</v>
-      </c>
-      <c r="F13" s="15">
+        <v>2718</v>
+      </c>
+      <c r="F13" s="8">
+        <f t="shared" si="8"/>
+        <v>375</v>
+      </c>
+      <c r="G13" s="23"/>
+      <c r="H13" s="34"/>
+      <c r="I13" s="27"/>
+      <c r="J13" s="9">
+        <f t="shared" si="7"/>
+        <v>1.1600512163892445</v>
+      </c>
+      <c r="K13" s="10">
+        <f t="shared" si="2"/>
+        <v>10.705423608649415</v>
+      </c>
+      <c r="L13" s="10">
+        <f t="shared" si="9"/>
+        <v>1.072111846946284</v>
+      </c>
+      <c r="M13" s="25"/>
+      <c r="AL13">
         <f t="shared" si="5"/>
-        <v>375</v>
-      </c>
-      <c r="G13" s="15">
-        <v>90</v>
-      </c>
-      <c r="H13" s="16">
-        <f t="shared" si="4"/>
-        <v>1.1984635083226634</v>
-      </c>
-      <c r="I13" s="17">
+        <v>900</v>
+      </c>
+      <c r="AN13">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="23"/>
+      <c r="C14" s="9">
+        <f t="shared" si="6"/>
+        <v>33.333333333333336</v>
+      </c>
+      <c r="D14" s="8">
+        <v>2343</v>
+      </c>
+      <c r="E14" s="8">
+        <f t="shared" si="0"/>
+        <v>2664</v>
+      </c>
+      <c r="F14" s="8">
+        <f t="shared" si="8"/>
+        <v>321</v>
+      </c>
+      <c r="G14" s="23"/>
+      <c r="H14" s="34"/>
+      <c r="I14" s="27"/>
+      <c r="J14" s="9">
+        <f t="shared" si="7"/>
+        <v>1.1370038412291934</v>
+      </c>
+      <c r="K14" s="10">
         <f t="shared" si="2"/>
-        <v>11.059907834101383</v>
-      </c>
-      <c r="J13" s="3"/>
-      <c r="AH13">
+        <v>10.492733073378234</v>
+      </c>
+      <c r="L14" s="10">
+        <f t="shared" si="9"/>
+        <v>1.0938438438438438</v>
+      </c>
+      <c r="M14" s="25"/>
+      <c r="AL14">
+        <f t="shared" si="5"/>
+        <v>1000</v>
+      </c>
+      <c r="AN14">
         <f t="shared" si="3"/>
-        <v>900</v>
-      </c>
-      <c r="AJ13">
-        <f xml:space="preserve"> F20 - F20*0.01*C21</f>
-        <v>0</v>
+        <v>259.15629999999999</v>
       </c>
     </row>
-    <row r="14" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B14" s="18"/>
-      <c r="C14" s="16">
-        <f>AH7/9</f>
-        <v>33.333333333333336</v>
-      </c>
-      <c r="D14" s="15">
+    <row r="15" spans="2:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="23"/>
+      <c r="C15" s="9">
+        <f t="shared" si="6"/>
+        <v>44.444444444444443</v>
+      </c>
+      <c r="D15" s="8">
         <v>2343</v>
       </c>
-      <c r="E14" s="15">
+      <c r="E15" s="8">
         <f t="shared" si="0"/>
-        <v>2754</v>
-      </c>
-      <c r="F14" s="15">
+        <v>2611</v>
+      </c>
+      <c r="F15" s="8">
+        <f t="shared" si="8"/>
+        <v>268</v>
+      </c>
+      <c r="G15" s="23"/>
+      <c r="H15" s="34"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="9">
+        <f t="shared" si="7"/>
+        <v>1.1143832693128468</v>
+      </c>
+      <c r="K15" s="10">
+        <f t="shared" si="2"/>
+        <v>10.283981251723187</v>
+      </c>
+      <c r="L15" s="10">
+        <f t="shared" si="9"/>
+        <v>1.1160474913826122</v>
+      </c>
+      <c r="M15" s="25"/>
+      <c r="AL15">
         <f t="shared" si="5"/>
-        <v>321</v>
-      </c>
-      <c r="G14" s="15">
-        <v>90</v>
-      </c>
-      <c r="H14" s="16">
-        <f t="shared" si="4"/>
-        <v>1.1754161331626121</v>
-      </c>
-      <c r="I14" s="17">
+        <v>1100</v>
+      </c>
+      <c r="AN15">
+        <f t="shared" si="3"/>
+        <v>173.42000000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="2:40" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="23"/>
+      <c r="C16" s="9">
+        <f t="shared" si="6"/>
+        <v>55.555555555555557</v>
+      </c>
+      <c r="D16" s="8">
+        <v>2343</v>
+      </c>
+      <c r="E16" s="8">
+        <f t="shared" si="0"/>
+        <v>2557</v>
+      </c>
+      <c r="F16" s="8">
+        <f t="shared" si="8"/>
+        <v>214</v>
+      </c>
+      <c r="G16" s="23"/>
+      <c r="H16" s="34"/>
+      <c r="I16" s="27"/>
+      <c r="J16" s="9">
+        <f t="shared" si="7"/>
+        <v>1.0913358941527955</v>
+      </c>
+      <c r="K16" s="10">
         <f t="shared" si="2"/>
-        <v>10.847217298830202</v>
-      </c>
-      <c r="J14" s="3"/>
-      <c r="AH14">
-        <f t="shared" si="3"/>
-        <v>1000</v>
-      </c>
-      <c r="AJ14">
-        <f xml:space="preserve"> F21 - F21*0.01*C22</f>
-        <v>259.15629999999999</v>
-      </c>
+        <v>10.071290716452006</v>
+      </c>
+      <c r="L16" s="10">
+        <f t="shared" si="9"/>
+        <v>1.1396167383652718</v>
+      </c>
+      <c r="M16" s="25"/>
     </row>
-    <row r="15" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B15" s="18"/>
-      <c r="C15" s="16">
-        <f>AH8/9</f>
-        <v>44.444444444444443</v>
-      </c>
-      <c r="D15" s="15">
+    <row r="17" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="23"/>
+      <c r="C17" s="9">
+        <f t="shared" si="6"/>
+        <v>66.666666666666671</v>
+      </c>
+      <c r="D17" s="8">
         <v>2343</v>
       </c>
-      <c r="E15" s="15">
+      <c r="E17" s="8">
         <f t="shared" si="0"/>
-        <v>2701</v>
-      </c>
-      <c r="F15" s="15">
-        <f t="shared" si="5"/>
-        <v>268</v>
-      </c>
-      <c r="G15" s="15">
-        <v>90</v>
-      </c>
-      <c r="H15" s="16">
-        <f t="shared" si="4"/>
-        <v>1.1527955612462655</v>
-      </c>
-      <c r="I15" s="17">
+        <v>2504</v>
+      </c>
+      <c r="F17" s="8">
+        <f t="shared" si="8"/>
+        <v>161</v>
+      </c>
+      <c r="G17" s="23"/>
+      <c r="H17" s="34"/>
+      <c r="I17" s="27"/>
+      <c r="J17" s="9">
+        <f t="shared" si="7"/>
+        <v>1.0687153222364489</v>
+      </c>
+      <c r="K17" s="10">
         <f t="shared" si="2"/>
-        <v>10.638465477175155</v>
-      </c>
-      <c r="J15" s="3"/>
-      <c r="AH15">
-        <f t="shared" si="3"/>
-        <v>1100</v>
-      </c>
-      <c r="AJ15">
-        <f xml:space="preserve"> F22 - F22*0.01*C23</f>
-        <v>173.42000000000002</v>
-      </c>
+        <v>9.8625388947969608</v>
+      </c>
+      <c r="L17" s="10">
+        <f t="shared" si="9"/>
+        <v>1.163738019169329</v>
+      </c>
+      <c r="M17" s="25"/>
     </row>
-    <row r="16" spans="2:36" x14ac:dyDescent="0.25">
-      <c r="B16" s="18"/>
-      <c r="C16" s="16">
-        <f>AH9/9</f>
-        <v>55.555555555555557</v>
-      </c>
-      <c r="D16" s="15">
+    <row r="18" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="23"/>
+      <c r="C18" s="9">
+        <f t="shared" si="6"/>
+        <v>77.777777777777771</v>
+      </c>
+      <c r="D18" s="8">
         <v>2343</v>
       </c>
-      <c r="E16" s="15">
+      <c r="E18" s="8">
         <f t="shared" si="0"/>
-        <v>2647</v>
-      </c>
-      <c r="F16" s="15">
-        <f t="shared" si="5"/>
-        <v>214</v>
-      </c>
-      <c r="G16" s="15">
-        <v>90</v>
-      </c>
-      <c r="H16" s="16">
-        <f t="shared" si="4"/>
-        <v>1.1297481860862142</v>
-      </c>
-      <c r="I16" s="17">
+        <v>2450</v>
+      </c>
+      <c r="F18" s="8">
+        <f t="shared" si="8"/>
+        <v>107</v>
+      </c>
+      <c r="G18" s="23"/>
+      <c r="H18" s="34"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="9">
+        <f t="shared" si="7"/>
+        <v>1.0456679470763979</v>
+      </c>
+      <c r="K18" s="10">
         <f t="shared" si="2"/>
-        <v>10.425774941903974</v>
-      </c>
-      <c r="J16" s="3"/>
+        <v>9.6498483595257802</v>
+      </c>
+      <c r="L18" s="10">
+        <f t="shared" si="9"/>
+        <v>1.1893877551020406</v>
+      </c>
+      <c r="M18" s="25"/>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B17" s="18"/>
-      <c r="C17" s="16">
-        <f>AH10/9</f>
-        <v>66.666666666666671</v>
-      </c>
-      <c r="D17" s="15">
+    <row r="19" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="23"/>
+      <c r="C19" s="9">
+        <f t="shared" si="6"/>
+        <v>88.888888888888886</v>
+      </c>
+      <c r="D19" s="8">
         <v>2343</v>
       </c>
-      <c r="E17" s="15">
+      <c r="E19" s="8">
         <f t="shared" si="0"/>
-        <v>2594</v>
-      </c>
-      <c r="F17" s="15">
-        <f t="shared" si="5"/>
-        <v>161</v>
-      </c>
-      <c r="G17" s="15">
-        <v>90</v>
-      </c>
-      <c r="H17" s="16">
-        <f t="shared" si="4"/>
-        <v>1.1071276141698676</v>
-      </c>
-      <c r="I17" s="17">
+        <v>2397</v>
+      </c>
+      <c r="F19" s="8">
+        <f t="shared" si="8"/>
+        <v>54</v>
+      </c>
+      <c r="G19" s="23"/>
+      <c r="H19" s="34"/>
+      <c r="I19" s="27"/>
+      <c r="J19" s="9">
+        <f t="shared" si="7"/>
+        <v>1.0230473751600513</v>
+      </c>
+      <c r="K19" s="10">
         <f t="shared" si="2"/>
-        <v>10.217023120248927</v>
-      </c>
-      <c r="J17" s="3"/>
+        <v>9.441096537870731</v>
+      </c>
+      <c r="L19" s="10">
+        <f t="shared" si="9"/>
+        <v>1.215686274509804</v>
+      </c>
+      <c r="M19" s="25"/>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B18" s="18"/>
-      <c r="C18" s="16">
-        <f>AH11/9</f>
-        <v>77.777777777777771</v>
-      </c>
-      <c r="D18" s="15">
-        <v>2343</v>
-      </c>
-      <c r="E18" s="15">
-        <f t="shared" si="0"/>
-        <v>2540</v>
-      </c>
-      <c r="F18" s="15">
-        <f t="shared" si="5"/>
-        <v>107</v>
-      </c>
-      <c r="G18" s="15">
-        <v>90</v>
-      </c>
-      <c r="H18" s="16">
-        <f t="shared" si="4"/>
-        <v>1.0840802390098165</v>
-      </c>
-      <c r="I18" s="17">
-        <f t="shared" si="2"/>
-        <v>10.004332584977746</v>
-      </c>
-      <c r="J18" s="3"/>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B19" s="18"/>
-      <c r="C19" s="16">
-        <f>AH12/9</f>
-        <v>88.888888888888886</v>
-      </c>
-      <c r="D19" s="15">
-        <v>2343</v>
-      </c>
-      <c r="E19" s="15">
-        <f t="shared" si="0"/>
-        <v>2487</v>
-      </c>
-      <c r="F19" s="15">
-        <f t="shared" si="5"/>
-        <v>54</v>
-      </c>
-      <c r="G19" s="15">
-        <v>90</v>
-      </c>
-      <c r="H19" s="16">
-        <f t="shared" si="4"/>
-        <v>1.0614596670934699</v>
-      </c>
-      <c r="I19" s="17">
-        <f t="shared" si="2"/>
-        <v>9.7955807633226986</v>
-      </c>
-      <c r="J19" s="3"/>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B20" s="19"/>
-      <c r="C20" s="14">
+    <row r="20" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="23"/>
+      <c r="C20" s="7">
         <f>100</f>
         <v>100</v>
       </c>
-      <c r="D20" s="15">
+      <c r="D20" s="8">
         <v>2343</v>
       </c>
-      <c r="E20" s="15">
+      <c r="E20" s="8">
         <f t="shared" si="0"/>
-        <v>2433</v>
-      </c>
-      <c r="F20" s="15">
+        <v>2343</v>
+      </c>
+      <c r="F20" s="8">
         <f>IF(ROUNDUP($F$11-$F$11*0.01*C20,0)&gt;0,ROUNDUP($F$11-$F$11*0.01*C20,0),0)</f>
         <v>0</v>
       </c>
-      <c r="G20" s="15">
-        <v>90</v>
-      </c>
-      <c r="H20" s="16">
-        <f t="shared" si="4"/>
-        <v>1.0384122919334187</v>
-      </c>
-      <c r="I20" s="17">
+      <c r="G20" s="23"/>
+      <c r="H20" s="35"/>
+      <c r="I20" s="27"/>
+      <c r="J20" s="9">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="K20" s="10">
         <f t="shared" si="2"/>
-        <v>9.582890228051518</v>
-      </c>
-      <c r="J20" s="3"/>
+        <v>9.2284060025995505</v>
+      </c>
+      <c r="L20" s="10">
+        <f t="shared" si="9"/>
+        <v>1.2437046521553565</v>
+      </c>
+      <c r="M20" s="25"/>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B21" s="20">
+    <row r="21" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="22">
         <v>3</v>
       </c>
-      <c r="C21" s="21">
+      <c r="C21" s="11">
         <v>0</v>
       </c>
-      <c r="D21" s="21">
+      <c r="D21" s="11">
         <v>1047</v>
       </c>
-      <c r="E21" s="21">
+      <c r="E21" s="11">
         <f t="shared" si="0"/>
         <v>1426</v>
       </c>
-      <c r="F21" s="21">
+      <c r="F21" s="11">
         <v>311</v>
       </c>
-      <c r="G21" s="21">
+      <c r="G21" s="22">
+        <v>279</v>
+      </c>
+      <c r="H21" s="36">
         <v>68</v>
       </c>
-      <c r="H21" s="22">
-        <f t="shared" si="4"/>
+      <c r="I21" s="28">
+        <f>(H21/G21)*100</f>
+        <v>24.372759856630825</v>
+      </c>
+      <c r="J21" s="12">
+        <f t="shared" si="7"/>
         <v>1.3619866284622733</v>
       </c>
-      <c r="I21" s="23">
+      <c r="K21" s="13">
         <f t="shared" si="2"/>
         <v>5.6166056166056171</v>
       </c>
-      <c r="J21" s="3"/>
+      <c r="L21" s="13">
+        <f>$K$21/K21</f>
+        <v>1</v>
+      </c>
+      <c r="M21" s="25"/>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B22" s="24"/>
-      <c r="C22" s="21">
+    <row r="22" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="22"/>
+      <c r="C22" s="11">
         <v>16.670000000000002</v>
       </c>
-      <c r="D22" s="21">
+      <c r="D22" s="11">
         <v>1047</v>
       </c>
-      <c r="E22" s="21">
+      <c r="E22" s="11">
         <f t="shared" si="0"/>
-        <v>1375</v>
-      </c>
-      <c r="F22" s="21">
-        <f t="shared" ref="F22:F27" si="6">ROUNDUP($F$21 - $F$21*0.01*C22,0)</f>
+        <v>1307</v>
+      </c>
+      <c r="F22" s="11">
+        <f t="shared" ref="F22:F27" si="10">ROUNDUP($F$21 - $F$21*0.01*C22,0)</f>
         <v>260</v>
       </c>
-      <c r="G22" s="21">
-        <v>68</v>
-      </c>
-      <c r="H22" s="22">
-        <f t="shared" si="4"/>
-        <v>1.3132760267430754</v>
-      </c>
-      <c r="I22" s="23">
+      <c r="G22" s="22"/>
+      <c r="H22" s="37"/>
+      <c r="I22" s="28"/>
+      <c r="J22" s="12">
+        <f t="shared" si="7"/>
+        <v>1.2483285577841452</v>
+      </c>
+      <c r="K22" s="13">
         <f t="shared" si="2"/>
-        <v>5.4157312221828349</v>
-      </c>
-      <c r="J22" s="3"/>
+        <v>5.1478986962857931</v>
+      </c>
+      <c r="L22" s="13">
+        <f t="shared" ref="L22:L27" si="11">$K$21/K22</f>
+        <v>1.0910482019892884</v>
+      </c>
+      <c r="M22" s="25"/>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B23" s="24"/>
-      <c r="C23" s="21">
+    <row r="23" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="22"/>
+      <c r="C23" s="11">
         <v>33.299999999999997</v>
       </c>
-      <c r="D23" s="21">
+      <c r="D23" s="11">
         <v>1047</v>
       </c>
-      <c r="E23" s="21">
+      <c r="E23" s="11">
         <f t="shared" si="0"/>
-        <v>1323</v>
-      </c>
-      <c r="F23" s="21">
-        <f t="shared" si="6"/>
+        <v>1255</v>
+      </c>
+      <c r="F23" s="11">
+        <f t="shared" si="10"/>
         <v>208</v>
       </c>
-      <c r="G23" s="21">
-        <v>68</v>
-      </c>
-      <c r="H23" s="22">
-        <f t="shared" si="4"/>
-        <v>1.2636103151862463</v>
-      </c>
-      <c r="I23" s="23">
+      <c r="G23" s="22"/>
+      <c r="H23" s="37"/>
+      <c r="I23" s="28"/>
+      <c r="J23" s="12">
+        <f t="shared" si="7"/>
+        <v>1.1986628462273161</v>
+      </c>
+      <c r="K23" s="13">
         <f t="shared" si="2"/>
-        <v>5.2109181141439205</v>
-      </c>
-      <c r="J23" s="3"/>
+        <v>4.9430855882468787</v>
+      </c>
+      <c r="L23" s="13">
+        <f t="shared" si="11"/>
+        <v>1.1362549800796813</v>
+      </c>
+      <c r="M23" s="25"/>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B24" s="24"/>
-      <c r="C24" s="21">
+    <row r="24" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="22"/>
+      <c r="C24" s="11">
         <v>50</v>
       </c>
-      <c r="D24" s="21">
+      <c r="D24" s="11">
         <v>1047</v>
       </c>
-      <c r="E24" s="21">
+      <c r="E24" s="11">
         <f t="shared" si="0"/>
-        <v>1271</v>
-      </c>
-      <c r="F24" s="21">
-        <f t="shared" si="6"/>
+        <v>1203</v>
+      </c>
+      <c r="F24" s="11">
+        <f t="shared" si="10"/>
         <v>156</v>
       </c>
-      <c r="G24" s="21">
-        <v>68</v>
-      </c>
-      <c r="H24" s="22">
-        <f t="shared" si="4"/>
-        <v>1.2139446036294175</v>
-      </c>
-      <c r="I24" s="23">
+      <c r="G24" s="22"/>
+      <c r="H24" s="37"/>
+      <c r="I24" s="28"/>
+      <c r="J24" s="12">
+        <f t="shared" si="7"/>
+        <v>1.148997134670487</v>
+      </c>
+      <c r="K24" s="13">
         <f t="shared" si="2"/>
-        <v>5.0061050061050061</v>
-      </c>
-      <c r="J24" s="3"/>
+        <v>4.7382724802079643</v>
+      </c>
+      <c r="L24" s="13">
+        <f t="shared" si="11"/>
+        <v>1.1853699085619285</v>
+      </c>
+      <c r="M24" s="25"/>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B25" s="24"/>
-      <c r="C25" s="21">
+    <row r="25" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="22"/>
+      <c r="C25" s="11">
         <v>66.599999999999994</v>
       </c>
-      <c r="D25" s="21">
+      <c r="D25" s="11">
         <v>1047</v>
       </c>
-      <c r="E25" s="21">
+      <c r="E25" s="11">
         <f t="shared" si="0"/>
-        <v>1219</v>
-      </c>
-      <c r="F25" s="21">
-        <f t="shared" si="6"/>
+        <v>1151</v>
+      </c>
+      <c r="F25" s="11">
+        <f t="shared" si="10"/>
         <v>104</v>
       </c>
-      <c r="G25" s="21">
-        <v>68</v>
-      </c>
-      <c r="H25" s="22">
-        <f t="shared" si="4"/>
-        <v>1.1642788920725884</v>
-      </c>
-      <c r="I25" s="23">
+      <c r="G25" s="22"/>
+      <c r="H25" s="37"/>
+      <c r="I25" s="28"/>
+      <c r="J25" s="12">
+        <f t="shared" si="7"/>
+        <v>1.0993314231136582</v>
+      </c>
+      <c r="K25" s="13">
         <f t="shared" si="2"/>
-        <v>4.8012918980660917</v>
-      </c>
-      <c r="J25" s="3"/>
+        <v>4.533459372169049</v>
+      </c>
+      <c r="L25" s="13">
+        <f t="shared" si="11"/>
+        <v>1.2389226759339707</v>
+      </c>
+      <c r="M25" s="25"/>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B26" s="24"/>
-      <c r="C26" s="21">
+    <row r="26" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="22"/>
+      <c r="C26" s="11">
         <v>83.3</v>
       </c>
-      <c r="D26" s="21">
+      <c r="D26" s="11">
         <v>1047</v>
       </c>
-      <c r="E26" s="21">
+      <c r="E26" s="11">
         <f t="shared" si="0"/>
-        <v>1167</v>
-      </c>
-      <c r="F26" s="21">
-        <f t="shared" si="6"/>
+        <v>1099</v>
+      </c>
+      <c r="F26" s="11">
+        <f t="shared" si="10"/>
         <v>52</v>
       </c>
-      <c r="G26" s="21">
-        <v>68</v>
-      </c>
-      <c r="H26" s="22">
-        <f t="shared" si="4"/>
-        <v>1.1146131805157593</v>
-      </c>
-      <c r="I26" s="23">
+      <c r="G26" s="22"/>
+      <c r="H26" s="37"/>
+      <c r="I26" s="28"/>
+      <c r="J26" s="12">
+        <f t="shared" si="7"/>
+        <v>1.0496657115568291</v>
+      </c>
+      <c r="K26" s="13">
         <f t="shared" si="2"/>
-        <v>4.5964787900271773</v>
-      </c>
-      <c r="J26" s="3"/>
+        <v>4.3286462641301346</v>
+      </c>
+      <c r="L26" s="13">
+        <f t="shared" si="11"/>
+        <v>1.2975432211101003</v>
+      </c>
+      <c r="M26" s="25"/>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B27" s="25"/>
-      <c r="C27" s="21">
+    <row r="27" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="22"/>
+      <c r="C27" s="11">
         <v>100</v>
       </c>
-      <c r="D27" s="21">
+      <c r="D27" s="11">
         <v>1047</v>
       </c>
-      <c r="E27" s="21">
+      <c r="E27" s="11">
         <f t="shared" si="0"/>
-        <v>1115</v>
-      </c>
-      <c r="F27" s="21">
-        <f t="shared" si="6"/>
+        <v>1047</v>
+      </c>
+      <c r="F27" s="11">
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="G27" s="21">
-        <v>68</v>
-      </c>
-      <c r="H27" s="22">
-        <f t="shared" si="4"/>
-        <v>1.0649474689589302</v>
-      </c>
-      <c r="I27" s="23">
+      <c r="G27" s="22"/>
+      <c r="H27" s="38"/>
+      <c r="I27" s="28"/>
+      <c r="J27" s="12">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="K27" s="13">
         <f t="shared" si="2"/>
-        <v>4.3916656819882629</v>
-      </c>
-      <c r="J27" s="4"/>
+        <v>4.1238331560912211</v>
+      </c>
+      <c r="L27" s="13">
+        <f t="shared" si="11"/>
+        <v>1.361986628462273</v>
+      </c>
+      <c r="M27" s="25"/>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B28" s="24">
+        <v>4</v>
+      </c>
+      <c r="C28" s="14">
+        <f>AL4/9</f>
+        <v>0</v>
+      </c>
+      <c r="D28" s="15">
+        <v>4014670</v>
+      </c>
+      <c r="E28" s="15">
+        <f t="shared" ref="E28:E37" si="12">D28+F28+H28</f>
+        <v>6613297</v>
+      </c>
+      <c r="F28" s="15">
+        <v>2447628</v>
+      </c>
+      <c r="G28" s="24">
+        <v>2656355</v>
+      </c>
+      <c r="H28" s="18">
+        <v>150999</v>
+      </c>
+      <c r="I28" s="29">
+        <f>(H28/G28)*100</f>
+        <v>5.6844435325850649</v>
+      </c>
+      <c r="J28" s="16">
+        <f t="shared" ref="J28:J37" si="13" xml:space="preserve"> E28/D28</f>
+        <v>1.6472828401836266</v>
+      </c>
+      <c r="K28" s="17">
+        <f t="shared" si="2"/>
+        <v>26047.88294143133</v>
+      </c>
+      <c r="L28" s="17">
+        <f>$K$28/K28</f>
+        <v>1</v>
+      </c>
+      <c r="M28" s="25"/>
+    </row>
+    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B29" s="24"/>
+      <c r="C29" s="16">
+        <f t="shared" ref="C29:C37" si="14">AL5/9</f>
+        <v>11.111111111111111</v>
+      </c>
+      <c r="D29" s="15">
+        <v>4014670</v>
+      </c>
+      <c r="E29" s="15">
+        <f t="shared" si="12"/>
+        <v>6190340</v>
+      </c>
+      <c r="F29" s="15">
+        <f>ROUNDUP($F$28 -$F$28*0.01*C29,0)</f>
+        <v>2175670</v>
+      </c>
+      <c r="G29" s="24"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="29"/>
+      <c r="J29" s="16">
+        <f t="shared" si="13"/>
+        <v>1.5419299718283197</v>
+      </c>
+      <c r="K29" s="17">
+        <f t="shared" si="2"/>
+        <v>24381.976446492576</v>
+      </c>
+      <c r="L29" s="17">
+        <f t="shared" ref="L29:L37" si="15">$K$28/K29</f>
+        <v>1.0683253262341004</v>
+      </c>
+      <c r="M29" s="25"/>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B30" s="24"/>
+      <c r="C30" s="16">
+        <f t="shared" si="14"/>
+        <v>22.222222222222221</v>
+      </c>
+      <c r="D30" s="15">
+        <v>4014670</v>
+      </c>
+      <c r="E30" s="15">
+        <f t="shared" si="12"/>
+        <v>5918381</v>
+      </c>
+      <c r="F30" s="15">
+        <f t="shared" ref="F30:F37" si="16">ROUNDUP($F$28 -$F$28*0.01*C30,0)</f>
+        <v>1903711</v>
+      </c>
+      <c r="G30" s="24"/>
+      <c r="H30" s="19"/>
+      <c r="I30" s="29"/>
+      <c r="J30" s="16">
+        <f t="shared" si="13"/>
+        <v>1.4741886630781609</v>
+      </c>
+      <c r="K30" s="17">
+        <f t="shared" si="2"/>
+        <v>23310.80783016267</v>
+      </c>
+      <c r="L30" s="17">
+        <f t="shared" si="15"/>
+        <v>1.1174165705114287</v>
+      </c>
+      <c r="M30" s="25"/>
+    </row>
+    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B31" s="24"/>
+      <c r="C31" s="16">
+        <f t="shared" si="14"/>
+        <v>33.333333333333336</v>
+      </c>
+      <c r="D31" s="15">
+        <v>4014670</v>
+      </c>
+      <c r="E31" s="15">
+        <f t="shared" si="12"/>
+        <v>5646422</v>
+      </c>
+      <c r="F31" s="15">
+        <f t="shared" si="16"/>
+        <v>1631752</v>
+      </c>
+      <c r="G31" s="24"/>
+      <c r="H31" s="19"/>
+      <c r="I31" s="29"/>
+      <c r="J31" s="16">
+        <f t="shared" si="13"/>
+        <v>1.4064473543280021</v>
+      </c>
+      <c r="K31" s="17">
+        <f t="shared" si="2"/>
+        <v>22239.639213832761</v>
+      </c>
+      <c r="L31" s="17">
+        <f t="shared" si="15"/>
+        <v>1.1712367584286121</v>
+      </c>
+      <c r="M31" s="25"/>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B32" s="24"/>
+      <c r="C32" s="16">
+        <f t="shared" si="14"/>
+        <v>44.444444444444443</v>
+      </c>
+      <c r="D32" s="15">
+        <v>4014670</v>
+      </c>
+      <c r="E32" s="15">
+        <f t="shared" si="12"/>
+        <v>5374464</v>
+      </c>
+      <c r="F32" s="15">
+        <f t="shared" si="16"/>
+        <v>1359794</v>
+      </c>
+      <c r="G32" s="24"/>
+      <c r="H32" s="19"/>
+      <c r="I32" s="29"/>
+      <c r="J32" s="16">
+        <f t="shared" si="13"/>
+        <v>1.3387062946643187</v>
+      </c>
+      <c r="K32" s="17">
+        <f t="shared" si="2"/>
+        <v>21168.474536216472</v>
+      </c>
+      <c r="L32" s="17">
+        <f t="shared" si="15"/>
+        <v>1.2305035441673813</v>
+      </c>
+      <c r="M32" s="25"/>
+    </row>
+    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B33" s="24"/>
+      <c r="C33" s="16">
+        <f t="shared" si="14"/>
+        <v>55.555555555555557</v>
+      </c>
+      <c r="D33" s="15">
+        <v>4014670</v>
+      </c>
+      <c r="E33" s="15">
+        <f t="shared" si="12"/>
+        <v>5102505</v>
+      </c>
+      <c r="F33" s="15">
+        <f t="shared" si="16"/>
+        <v>1087835</v>
+      </c>
+      <c r="G33" s="24"/>
+      <c r="H33" s="19"/>
+      <c r="I33" s="29"/>
+      <c r="J33" s="16">
+        <f t="shared" si="13"/>
+        <v>1.2709649859141599</v>
+      </c>
+      <c r="K33" s="17">
+        <f t="shared" si="2"/>
+        <v>20097.305919886563</v>
+      </c>
+      <c r="L33" s="17">
+        <f t="shared" si="15"/>
+        <v>1.2960882938870224</v>
+      </c>
+      <c r="M33" s="25"/>
+    </row>
+    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B34" s="24"/>
+      <c r="C34" s="16">
+        <f t="shared" si="14"/>
+        <v>66.666666666666671</v>
+      </c>
+      <c r="D34" s="15">
+        <v>4014670</v>
+      </c>
+      <c r="E34" s="15">
+        <f t="shared" si="12"/>
+        <v>4830546</v>
+      </c>
+      <c r="F34" s="15">
+        <f t="shared" si="16"/>
+        <v>815876</v>
+      </c>
+      <c r="G34" s="24"/>
+      <c r="H34" s="19"/>
+      <c r="I34" s="29"/>
+      <c r="J34" s="16">
+        <f t="shared" si="13"/>
+        <v>1.203223677164001</v>
+      </c>
+      <c r="K34" s="17">
+        <f t="shared" si="2"/>
+        <v>19026.137303556658</v>
+      </c>
+      <c r="L34" s="17">
+        <f t="shared" si="15"/>
+        <v>1.369057866336435</v>
+      </c>
+      <c r="M34" s="25"/>
+    </row>
+    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B35" s="24"/>
+      <c r="C35" s="16">
+        <f t="shared" si="14"/>
+        <v>77.777777777777771</v>
+      </c>
+      <c r="D35" s="15">
+        <v>4014670</v>
+      </c>
+      <c r="E35" s="15">
+        <f t="shared" si="12"/>
+        <v>4558588</v>
+      </c>
+      <c r="F35" s="15">
+        <f t="shared" si="16"/>
+        <v>543918</v>
+      </c>
+      <c r="G35" s="24"/>
+      <c r="H35" s="19"/>
+      <c r="I35" s="29"/>
+      <c r="J35" s="16">
+        <f t="shared" si="13"/>
+        <v>1.1354826175003176</v>
+      </c>
+      <c r="K35" s="17">
+        <f t="shared" si="2"/>
+        <v>17954.972625940365</v>
+      </c>
+      <c r="L35" s="17">
+        <f t="shared" si="15"/>
+        <v>1.4507336482261615</v>
+      </c>
+      <c r="M35" s="25"/>
+    </row>
+    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B36" s="24"/>
+      <c r="C36" s="16">
+        <f t="shared" si="14"/>
+        <v>88.888888888888886</v>
+      </c>
+      <c r="D36" s="15">
+        <v>4014670</v>
+      </c>
+      <c r="E36" s="15">
+        <f t="shared" si="12"/>
+        <v>4286629</v>
+      </c>
+      <c r="F36" s="15">
+        <f t="shared" si="16"/>
+        <v>271959</v>
+      </c>
+      <c r="G36" s="24"/>
+      <c r="H36" s="19"/>
+      <c r="I36" s="29"/>
+      <c r="J36" s="16">
+        <f t="shared" si="13"/>
+        <v>1.0677413087501588</v>
+      </c>
+      <c r="K36" s="17">
+        <f t="shared" si="2"/>
+        <v>16883.80400961046</v>
+      </c>
+      <c r="L36" s="17">
+        <f t="shared" si="15"/>
+        <v>1.5427733540737958</v>
+      </c>
+      <c r="M36" s="25"/>
+    </row>
+    <row r="37" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B37" s="24"/>
+      <c r="C37" s="14">
+        <f t="shared" si="14"/>
+        <v>100</v>
+      </c>
+      <c r="D37" s="15">
+        <v>4014670</v>
+      </c>
+      <c r="E37" s="15">
+        <f t="shared" si="12"/>
+        <v>4014670</v>
+      </c>
+      <c r="F37" s="15">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="G37" s="24"/>
+      <c r="H37" s="20"/>
+      <c r="I37" s="29"/>
+      <c r="J37" s="16">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="K37" s="17">
+        <f t="shared" si="2"/>
+        <v>15812.635393280556</v>
+      </c>
+      <c r="L37" s="17">
+        <f t="shared" si="15"/>
+        <v>1.6472828401836264</v>
+      </c>
+      <c r="M37" s="25"/>
+    </row>
+    <row r="74" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C74">
+        <f>90/521</f>
+        <v>0.17274472168905949</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="17">
+    <mergeCell ref="M4:M37"/>
+    <mergeCell ref="I4:I10"/>
+    <mergeCell ref="I11:I20"/>
+    <mergeCell ref="I21:I27"/>
+    <mergeCell ref="I28:I37"/>
+    <mergeCell ref="H28:H37"/>
     <mergeCell ref="B4:B10"/>
     <mergeCell ref="B21:B27"/>
     <mergeCell ref="B11:B20"/>
-    <mergeCell ref="J4:J27"/>
+    <mergeCell ref="B28:B37"/>
+    <mergeCell ref="G21:G27"/>
+    <mergeCell ref="G11:G20"/>
+    <mergeCell ref="G4:G10"/>
+    <mergeCell ref="G28:G37"/>
+    <mergeCell ref="H4:H10"/>
+    <mergeCell ref="H11:H20"/>
+    <mergeCell ref="H21:H27"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="95" orientation="landscape" r:id="rId1"/>
+  <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="8" scale="60" fitToWidth="5" fitToHeight="5" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>